<commit_message>
Add user controlled bias for generating worst performing queries in WorstQueriesReport.sql plus fix query count in other reports
</commit_message>
<xml_diff>
--- a/QueryStore/SQLServer2016/ExcelTemplates/PerformanceReport.xlsx
+++ b/QueryStore/SQLServer2016/ExcelTemplates/PerformanceReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Version Control\SQLServerPerformanceTuning\QueryStore\SQLServer2016\ExcelTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24134ADC-93E8-41EC-B663-D44C1E99818C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6EA21B4-E1CF-4DD6-9D46-C3993BC05BAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" activeTab="7" xr2:uid="{E57F5ADB-DFB2-48C1-AB7B-5552241A8B93}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{E57F5ADB-DFB2-48C1-AB7B-5552241A8B93}"/>
   </bookViews>
   <sheets>
     <sheet name="PerformanceCharts" sheetId="16" r:id="rId1"/>
@@ -29,14 +29,16 @@
     <sheet name="Physical Reads" sheetId="44" r:id="rId14"/>
     <sheet name="Logical Writes" sheetId="48" r:id="rId15"/>
     <sheet name="Worst Performing Queries" sheetId="11" r:id="rId16"/>
-    <sheet name="Worst Queries by Plan Id" sheetId="12" r:id="rId17"/>
+    <sheet name="Worst Performing Plans" sheetId="53" r:id="rId17"/>
+    <sheet name="Worst Plan Stats" sheetId="12" r:id="rId18"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">'Worst Performing Plans'!#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">'Worst Performing Queries'!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="74" r:id="rId18"/>
+    <pivotCache cacheId="595" r:id="rId19"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -398,7 +400,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -407,7 +409,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -425,26 +426,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="129">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -537,6 +518,26 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -48129,7 +48130,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6B74A5C7-4412-4D02-A585-F29DACEC11A2}" name="PivotTable2" cacheId="74" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6B74A5C7-4412-4D02-A585-F29DACEC11A2}" name="PivotTable2" cacheId="595" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7">
   <location ref="A1:C4" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="25">
     <pivotField axis="axisCol" showAll="0">
@@ -48652,7 +48653,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{05205779-AA59-4F6D-B5B7-B5805E83743E}" name="PivotTable5" cacheId="74" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{05205779-AA59-4F6D-B5B7-B5805E83743E}" name="PivotTable5" cacheId="595" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
   <location ref="A3:C6" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="25">
     <pivotField axis="axisCol" showAll="0">
@@ -49166,7 +49167,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{18777F2B-B005-42C4-8BA6-420B837E756F}" name="PivotTable2" cacheId="74" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{18777F2B-B005-42C4-8BA6-420B837E756F}" name="PivotTable2" cacheId="595" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="A1:C4" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="25">
     <pivotField axis="axisCol" showAll="0">
@@ -49677,7 +49678,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A47CD3EC-D199-4326-A3BB-466C9182D620}" name="PivotTable2" cacheId="74" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A47CD3EC-D199-4326-A3BB-466C9182D620}" name="PivotTable2" cacheId="595" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8">
   <location ref="A1:C4" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="25">
     <pivotField axis="axisCol" showAll="0">
@@ -50197,7 +50198,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8950B02F-B669-42A6-B730-5717AEFF6DC1}" name="PivotTable3" cacheId="74" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8950B02F-B669-42A6-B730-5717AEFF6DC1}" name="PivotTable3" cacheId="595" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="A1:C4" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="25">
     <pivotField axis="axisCol" showAll="0">
@@ -50708,7 +50709,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DF2C72FF-63FA-483C-9CB9-93C4252E7C29}" name="PivotTable4" cacheId="74" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DF2C72FF-63FA-483C-9CB9-93C4252E7C29}" name="PivotTable4" cacheId="595" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="A1:C4" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="25">
     <pivotField axis="axisCol" showAll="0">
@@ -51349,52 +51350,52 @@
   <tableColumns count="3">
     <tableColumn id="25" xr3:uid="{F6AFC3C5-64F0-4AAE-A7AC-488DDD813EB0}" name="Database Name" dataDxfId="27"/>
     <tableColumn id="9" xr3:uid="{7D839B69-6D13-40A6-A83A-71FE946D8365}" name="Query Hash" dataDxfId="26"/>
-    <tableColumn id="1" xr3:uid="{9395593E-E1D7-4B2E-8FB8-52A3AD32CCEF}" name="capture_sql_statement" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{9395593E-E1D7-4B2E-8FB8-52A3AD32CCEF}" name="capture_sql_statement" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{182704C9-F0AE-4D54-B9C5-268D10F9597C}" name="Table12" displayName="Table12" ref="A4:D5" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A4:D5" xr:uid="{1053790E-AC77-4E52-971B-71D3B9221D89}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:C5">
-    <sortCondition ref="B5"/>
-    <sortCondition ref="C5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D0EB994C-0990-4D58-94D8-163A54D47F25}" name="Table123" displayName="Table123" ref="A1:D2" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A1:D2" xr:uid="{1053790E-AC77-4E52-971B-71D3B9221D89}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B2">
+    <sortCondition ref="A2"/>
+    <sortCondition ref="B2"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="5" xr3:uid="{4C4B65D8-ACD0-4866-A366-6C9DDBDC7711}" name="Database Name"/>
-    <tableColumn id="1" xr3:uid="{3BB94C17-1DF8-4460-905F-88C9F019E0DF}" name="Query Hash"/>
-    <tableColumn id="2" xr3:uid="{6C3C67E0-B7B2-4D0A-84A0-51D102BA1D3D}" name="Query Plan Hash"/>
-    <tableColumn id="3" xr3:uid="{748194F6-2EBD-4A7D-B716-85520B9A16AC}" name="capture_plan_statement"/>
+    <tableColumn id="5" xr3:uid="{F64E1AD0-977E-46ED-BD23-BAE360C228FB}" name="Database Name"/>
+    <tableColumn id="1" xr3:uid="{027DAB7E-8F78-4A5D-A8F6-595870860171}" name="Query Hash"/>
+    <tableColumn id="2" xr3:uid="{5C6239D3-CE63-4CF9-988E-156BD2B115F0}" name="Query Plan Hash"/>
+    <tableColumn id="3" xr3:uid="{6F092FCC-5733-4B94-872E-90EB037F2C2A}" name="capture_plan_statement"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{7670AAE7-476C-4ED1-BCF9-CF3EC7E34768}" name="Table13" displayName="Table13" ref="A1:P3" insertRow="1" totalsRowCount="1" headerRowDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{7670AAE7-476C-4ED1-BCF9-CF3EC7E34768}" name="Table13" displayName="Table13" ref="A1:P3" insertRow="1" totalsRowCount="1" headerRowDxfId="24">
   <autoFilter ref="A1:P2" xr:uid="{BA2BC664-8FDD-4485-A867-25558324D9E2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P2">
     <sortCondition ref="D2"/>
   </sortState>
   <tableColumns count="16">
-    <tableColumn id="17" xr3:uid="{BC04EF40-794A-476D-BEE5-3C16A645EAF3}" name="Database Name" dataDxfId="24"/>
-    <tableColumn id="1" xr3:uid="{6F27793A-6D96-4332-AF8F-E214B397B4F6}" name="Query Hash" dataDxfId="23"/>
+    <tableColumn id="17" xr3:uid="{BC04EF40-794A-476D-BEE5-3C16A645EAF3}" name="Database Name" dataDxfId="23"/>
+    <tableColumn id="1" xr3:uid="{6F27793A-6D96-4332-AF8F-E214B397B4F6}" name="Query Hash" dataDxfId="22"/>
     <tableColumn id="2" xr3:uid="{5F7491E8-CC8E-4368-A40E-446D31A439F3}" name="Object Name"/>
     <tableColumn id="3" xr3:uid="{20EA2CD5-9AD0-4947-A761-88F21BB15DB2}" name="Query Plan Hash"/>
     <tableColumn id="4" xr3:uid="{90343523-F827-4B71-9FFD-89EA58E217AD}" name="Execution Count"/>
-    <tableColumn id="5" xr3:uid="{3CAE4964-54EA-45F8-94F8-B0876F39FA5E}" name="Average Rowcount" dataDxfId="22" totalsRowDxfId="21"/>
-    <tableColumn id="18" xr3:uid="{49D47F76-708A-41B6-8C33-FE8F105CF42B}" name="Average Duration Microseconds" totalsRowFunction="average" dataDxfId="20" totalsRowDxfId="19"/>
-    <tableColumn id="8" xr3:uid="{778BF87D-30CB-4ED1-8957-95B635F027F5}" name="Total Duration Minutes" totalsRowFunction="sum" dataDxfId="18" totalsRowDxfId="17"/>
-    <tableColumn id="9" xr3:uid="{A9CF50FA-1B16-42B8-B627-BE7E5221D305}" name="Total CPU_x000a_Minutes" totalsRowFunction="sum" dataDxfId="16" totalsRowDxfId="15"/>
-    <tableColumn id="19" xr3:uid="{2B56BDB9-2B16-44CF-B58E-16BE8B5A4CFA}" name="Total CLR Minutes" totalsRowFunction="sum" dataDxfId="14" totalsRowDxfId="13"/>
-    <tableColumn id="20" xr3:uid="{CADFC995-67D2-412F-94C5-91A7749B6B29}" name="Average DoP" totalsRowFunction="average" dataDxfId="12" totalsRowDxfId="11"/>
-    <tableColumn id="10" xr3:uid="{0F8D4B6E-380C-4BE9-A80B-617917136E09}" name="Total Logical Reads GB" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="9"/>
-    <tableColumn id="13" xr3:uid="{AB515164-576B-4E0B-9DF8-91E2F202918A}" name="Total Memory Grants GB" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="7"/>
-    <tableColumn id="11" xr3:uid="{9A27FFF2-67DC-4BB4-B9FF-157529ACCC80}" name="Total Physical Reads GB" totalsRowFunction="sum" dataDxfId="6" totalsRowDxfId="5"/>
-    <tableColumn id="12" xr3:uid="{D61BAAD1-B446-42BB-BFDF-5418C86C241A}" name="Total Logical Writes GB" totalsRowFunction="sum" dataDxfId="4" totalsRowDxfId="3"/>
-    <tableColumn id="14" xr3:uid="{2C29A776-7BAF-4270-AF5C-05E32BA8316D}" name="Comment" dataDxfId="2" totalsRowDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{3CAE4964-54EA-45F8-94F8-B0876F39FA5E}" name="Average Rowcount" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="18" xr3:uid="{49D47F76-708A-41B6-8C33-FE8F105CF42B}" name="Average Duration Microseconds" totalsRowFunction="average" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="8" xr3:uid="{778BF87D-30CB-4ED1-8957-95B635F027F5}" name="Total Duration Minutes" totalsRowFunction="sum" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="9" xr3:uid="{A9CF50FA-1B16-42B8-B627-BE7E5221D305}" name="Total CPU_x000a_Minutes" totalsRowFunction="sum" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="19" xr3:uid="{2B56BDB9-2B16-44CF-B58E-16BE8B5A4CFA}" name="Total CLR Minutes" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="20" xr3:uid="{CADFC995-67D2-412F-94C5-91A7749B6B29}" name="Average DoP" totalsRowFunction="average" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="10" xr3:uid="{0F8D4B6E-380C-4BE9-A80B-617917136E09}" name="Total Logical Reads GB" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="13" xr3:uid="{AB515164-576B-4E0B-9DF8-91E2F202918A}" name="Total Memory Grants GB" totalsRowFunction="sum" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="11" xr3:uid="{9A27FFF2-67DC-4BB4-B9FF-157529ACCC80}" name="Total Physical Reads GB" totalsRowFunction="sum" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="12" xr3:uid="{D61BAAD1-B446-42BB-BFDF-5418C86C241A}" name="Total Logical Writes GB" totalsRowFunction="sum" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="14" xr3:uid="{2C29A776-7BAF-4270-AF5C-05E32BA8316D}" name="Comment" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -51832,7 +51833,7 @@
       <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -51844,22 +51845,24 @@
   <dimension ref="A1:K54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="23.26953125" customWidth="1"/>
-    <col min="3" max="3" width="38.90625" customWidth="1"/>
-    <col min="4" max="4" width="25.36328125" customWidth="1"/>
-    <col min="5" max="8" width="21.81640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="38.85546875" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20" style="1" customWidth="1"/>
-    <col min="10" max="10" width="15.26953125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
@@ -51872,18 +51875,18 @@
       <c r="D1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
     </row>
-    <row r="4" spans="1:11" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>24</v>
       </c>
@@ -51896,225 +51899,225 @@
       <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="J4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="K4" s="10" t="s">
+      <c r="K4" s="9" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D5" s="4"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D6" s="4"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D7" s="4"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D8" s="4"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D9" s="4"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D10" s="4"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D11" s="4"/>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D12" s="4"/>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D13" s="4"/>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D14" s="4"/>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D15" s="4"/>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D16" s="4"/>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="4:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D17" s="4"/>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="4:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D18" s="4"/>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="4:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D19" s="4"/>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="4:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D20" s="4"/>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="4:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D21" s="4"/>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="4:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D22" s="4"/>
       <c r="K22" s="1"/>
     </row>
-    <row r="23" spans="4:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D23" s="4"/>
       <c r="K23" s="1"/>
     </row>
-    <row r="24" spans="4:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D24" s="4"/>
       <c r="K24" s="1"/>
     </row>
-    <row r="25" spans="4:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D25" s="4"/>
       <c r="K25" s="1"/>
     </row>
-    <row r="26" spans="4:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D26" s="4"/>
       <c r="K26" s="1"/>
     </row>
-    <row r="27" spans="4:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D27" s="4"/>
       <c r="K27" s="1"/>
     </row>
-    <row r="28" spans="4:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D28" s="4"/>
       <c r="K28" s="1"/>
     </row>
-    <row r="29" spans="4:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D29" s="4"/>
       <c r="K29" s="1"/>
     </row>
-    <row r="30" spans="4:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D30" s="4"/>
       <c r="K30" s="1"/>
     </row>
-    <row r="31" spans="4:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D31" s="4"/>
       <c r="K31" s="1"/>
     </row>
-    <row r="32" spans="4:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D32" s="4"/>
       <c r="K32" s="1"/>
     </row>
-    <row r="33" spans="4:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D33" s="4"/>
       <c r="K33" s="1"/>
     </row>
-    <row r="34" spans="4:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D34" s="4"/>
       <c r="K34" s="1"/>
     </row>
-    <row r="35" spans="4:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D35" s="4"/>
       <c r="K35" s="1"/>
     </row>
-    <row r="36" spans="4:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D36" s="4"/>
       <c r="K36" s="1"/>
     </row>
-    <row r="37" spans="4:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D37" s="4"/>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="4:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D38" s="4"/>
       <c r="K38" s="1"/>
     </row>
-    <row r="39" spans="4:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D39" s="4"/>
       <c r="K39" s="1"/>
     </row>
-    <row r="40" spans="4:11" x14ac:dyDescent="0.35">
+    <row r="40" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D40" s="4"/>
       <c r="K40" s="1"/>
     </row>
-    <row r="41" spans="4:11" x14ac:dyDescent="0.35">
+    <row r="41" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D41" s="4"/>
       <c r="K41" s="1"/>
     </row>
-    <row r="42" spans="4:11" x14ac:dyDescent="0.35">
+    <row r="42" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D42" s="4"/>
       <c r="K42" s="1"/>
     </row>
-    <row r="43" spans="4:11" x14ac:dyDescent="0.35">
+    <row r="43" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D43" s="4"/>
       <c r="K43" s="1"/>
     </row>
-    <row r="44" spans="4:11" x14ac:dyDescent="0.35">
+    <row r="44" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D44" s="4"/>
       <c r="K44" s="1"/>
     </row>
-    <row r="45" spans="4:11" x14ac:dyDescent="0.35">
+    <row r="45" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D45" s="4"/>
       <c r="K45" s="1"/>
     </row>
-    <row r="46" spans="4:11" x14ac:dyDescent="0.35">
+    <row r="46" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D46" s="4"/>
       <c r="K46" s="1"/>
     </row>
-    <row r="47" spans="4:11" x14ac:dyDescent="0.35">
+    <row r="47" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D47" s="4"/>
       <c r="K47" s="1"/>
     </row>
-    <row r="48" spans="4:11" x14ac:dyDescent="0.35">
+    <row r="48" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D48" s="4"/>
       <c r="K48" s="1"/>
     </row>
-    <row r="49" spans="4:11" x14ac:dyDescent="0.35">
+    <row r="49" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D49" s="4"/>
       <c r="K49" s="1"/>
     </row>
-    <row r="50" spans="4:11" x14ac:dyDescent="0.35">
+    <row r="50" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D50" s="4"/>
       <c r="K50" s="1"/>
     </row>
-    <row r="51" spans="4:11" x14ac:dyDescent="0.35">
+    <row r="51" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D51" s="4"/>
       <c r="K51" s="1"/>
     </row>
-    <row r="52" spans="4:11" x14ac:dyDescent="0.35">
+    <row r="52" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D52" s="4"/>
       <c r="K52" s="1"/>
     </row>
-    <row r="53" spans="4:11" x14ac:dyDescent="0.35">
+    <row r="53" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D53" s="4"/>
       <c r="K53" s="1"/>
     </row>
-    <row r="54" spans="4:11" x14ac:dyDescent="0.35">
+    <row r="54" spans="4:11" x14ac:dyDescent="0.25">
       <c r="D54" s="4"/>
       <c r="K54" s="1"/>
     </row>
@@ -52133,22 +52136,24 @@
   <dimension ref="A1:J54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="23.26953125" customWidth="1"/>
-    <col min="3" max="3" width="38.90625" customWidth="1"/>
-    <col min="4" max="4" width="25.36328125" customWidth="1"/>
-    <col min="5" max="7" width="21.81640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="22.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20" style="1" customWidth="1"/>
-    <col min="10" max="10" width="15.26953125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="38.85546875" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>35</v>
       </c>
@@ -52161,18 +52166,18 @@
       <c r="D1" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
     </row>
-    <row r="4" spans="1:10" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>24</v>
       </c>
@@ -52185,173 +52190,173 @@
       <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I4" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="J4" s="9" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D9" s="4"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D12" s="4"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D13" s="4"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D14" s="4"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D15" s="4"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D16" s="4"/>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17" s="4"/>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D18" s="4"/>
     </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D19" s="4"/>
     </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D20" s="4"/>
     </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D21" s="4"/>
     </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D22" s="4"/>
     </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D23" s="4"/>
     </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D24" s="4"/>
     </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D25" s="4"/>
     </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D26" s="4"/>
     </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D27" s="4"/>
     </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D28" s="4"/>
     </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D29" s="4"/>
     </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D30" s="4"/>
     </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D31" s="4"/>
     </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D32" s="4"/>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D33" s="4"/>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D34" s="4"/>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D35" s="4"/>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D36" s="4"/>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D37" s="4"/>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D38" s="4"/>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D39" s="4"/>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D40" s="4"/>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D41" s="4"/>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D42" s="4"/>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D43" s="4"/>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D44" s="4"/>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D45" s="4"/>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D46" s="4"/>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D47" s="4"/>
     </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D48" s="4"/>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D49" s="4"/>
     </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D50" s="4"/>
     </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D51" s="4"/>
     </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D52" s="4"/>
     </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D53" s="4"/>
     </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D54" s="4"/>
     </row>
   </sheetData>
@@ -52369,21 +52374,23 @@
   <dimension ref="A1:J54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="23.26953125" customWidth="1"/>
-    <col min="3" max="3" width="38.90625" customWidth="1"/>
-    <col min="4" max="4" width="25.36328125" customWidth="1"/>
-    <col min="5" max="8" width="21.81640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="22.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.26953125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="38.85546875" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="23" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -52396,18 +52403,18 @@
       <c r="D1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
     </row>
-    <row r="4" spans="1:10" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>24</v>
       </c>
@@ -52420,173 +52427,173 @@
       <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="J4" s="9" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D9" s="4"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D12" s="4"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D13" s="4"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D14" s="4"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D15" s="4"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D16" s="4"/>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17" s="4"/>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D18" s="4"/>
     </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D19" s="4"/>
     </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D20" s="4"/>
     </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D21" s="4"/>
     </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D22" s="4"/>
     </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D23" s="4"/>
     </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D24" s="4"/>
     </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D25" s="4"/>
     </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D26" s="4"/>
     </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D27" s="4"/>
     </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D28" s="4"/>
     </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D29" s="4"/>
     </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D30" s="4"/>
     </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D31" s="4"/>
     </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D32" s="4"/>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D33" s="4"/>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D34" s="4"/>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D35" s="4"/>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D36" s="4"/>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D37" s="4"/>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D38" s="4"/>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D39" s="4"/>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D40" s="4"/>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D41" s="4"/>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D42" s="4"/>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D43" s="4"/>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D44" s="4"/>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D45" s="4"/>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D46" s="4"/>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D47" s="4"/>
     </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D48" s="4"/>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D49" s="4"/>
     </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D50" s="4"/>
     </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D51" s="4"/>
     </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D52" s="4"/>
     </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D53" s="4"/>
     </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D54" s="4"/>
     </row>
   </sheetData>
@@ -52607,21 +52614,21 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="23.26953125" customWidth="1"/>
-    <col min="3" max="3" width="38.90625" customWidth="1"/>
-    <col min="4" max="4" width="25.36328125" customWidth="1"/>
-    <col min="5" max="5" width="21.81640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="23.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.81640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="23.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20" style="1" customWidth="1"/>
-    <col min="10" max="10" width="17.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="38.85546875" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>32</v>
       </c>
@@ -52634,18 +52641,18 @@
       <c r="D1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
     </row>
-    <row r="4" spans="1:10" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>24</v>
       </c>
@@ -52658,173 +52665,173 @@
       <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I4" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="J4" s="9" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D9" s="4"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D12" s="4"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D13" s="4"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D14" s="4"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D15" s="4"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D16" s="4"/>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17" s="4"/>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D18" s="4"/>
     </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D19" s="4"/>
     </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D20" s="4"/>
     </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D21" s="4"/>
     </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D22" s="4"/>
     </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D23" s="4"/>
     </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D24" s="4"/>
     </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D25" s="4"/>
     </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D26" s="4"/>
     </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D27" s="4"/>
     </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D28" s="4"/>
     </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D29" s="4"/>
     </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D30" s="4"/>
     </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D31" s="4"/>
     </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D32" s="4"/>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D33" s="4"/>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D34" s="4"/>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D35" s="4"/>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D36" s="4"/>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D37" s="4"/>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D38" s="4"/>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D39" s="4"/>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D40" s="4"/>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D41" s="4"/>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D42" s="4"/>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D43" s="4"/>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D44" s="4"/>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D45" s="4"/>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D46" s="4"/>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D47" s="4"/>
     </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D48" s="4"/>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D49" s="4"/>
     </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D50" s="4"/>
     </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D51" s="4"/>
     </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D52" s="4"/>
     </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D53" s="4"/>
     </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D54" s="4"/>
     </row>
   </sheetData>
@@ -52845,20 +52852,20 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="23.26953125" customWidth="1"/>
-    <col min="3" max="3" width="38.90625" customWidth="1"/>
-    <col min="4" max="4" width="25.36328125" customWidth="1"/>
-    <col min="5" max="5" width="21.81640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="23.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.453125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="17.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="38.85546875" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>16</v>
       </c>
@@ -52871,18 +52878,18 @@
       <c r="D1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
     </row>
-    <row r="4" spans="1:10" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>24</v>
       </c>
@@ -52895,173 +52902,173 @@
       <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="J4" s="9" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D9" s="4"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D12" s="4"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D13" s="4"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D14" s="4"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D15" s="4"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D16" s="4"/>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17" s="4"/>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D18" s="4"/>
     </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D19" s="4"/>
     </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D20" s="4"/>
     </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D21" s="4"/>
     </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D22" s="4"/>
     </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D23" s="4"/>
     </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D24" s="4"/>
     </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D25" s="4"/>
     </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D26" s="4"/>
     </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D27" s="4"/>
     </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D28" s="4"/>
     </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D29" s="4"/>
     </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D30" s="4"/>
     </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D31" s="4"/>
     </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D32" s="4"/>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D33" s="4"/>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D34" s="4"/>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D35" s="4"/>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D36" s="4"/>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D37" s="4"/>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D38" s="4"/>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D39" s="4"/>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D40" s="4"/>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D41" s="4"/>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D42" s="4"/>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D43" s="4"/>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D44" s="4"/>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D45" s="4"/>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D46" s="4"/>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D47" s="4"/>
     </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D48" s="4"/>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D49" s="4"/>
     </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D50" s="4"/>
     </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D51" s="4"/>
     </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D52" s="4"/>
     </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D53" s="4"/>
     </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D54" s="4"/>
     </row>
   </sheetData>
@@ -53082,20 +53089,20 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="23.26953125" customWidth="1"/>
-    <col min="3" max="3" width="38.90625" customWidth="1"/>
-    <col min="4" max="4" width="25.36328125" customWidth="1"/>
-    <col min="5" max="5" width="19.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="22.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20" style="1" customWidth="1"/>
-    <col min="10" max="10" width="17.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="38.85546875" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
@@ -53108,18 +53115,18 @@
       <c r="D1" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
     </row>
-    <row r="4" spans="1:10" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>24</v>
       </c>
@@ -53132,173 +53139,173 @@
       <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I4" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="J4" s="9" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D9" s="4"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D12" s="4"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D13" s="4"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D14" s="4"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D15" s="4"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D16" s="4"/>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17" s="4"/>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D18" s="4"/>
     </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D19" s="4"/>
     </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D20" s="4"/>
     </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D21" s="4"/>
     </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D22" s="4"/>
     </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D23" s="4"/>
     </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D24" s="4"/>
     </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D25" s="4"/>
     </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D26" s="4"/>
     </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D27" s="4"/>
     </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D28" s="4"/>
     </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D29" s="4"/>
     </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D30" s="4"/>
     </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D31" s="4"/>
     </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D32" s="4"/>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D33" s="4"/>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D34" s="4"/>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D35" s="4"/>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D36" s="4"/>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D37" s="4"/>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D38" s="4"/>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D39" s="4"/>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D40" s="4"/>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D41" s="4"/>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D42" s="4"/>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D43" s="4"/>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D44" s="4"/>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D45" s="4"/>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D46" s="4"/>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D47" s="4"/>
     </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D48" s="4"/>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D49" s="4"/>
     </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D50" s="4"/>
     </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D51" s="4"/>
     </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D52" s="4"/>
     </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D53" s="4"/>
     </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D54" s="4"/>
     </row>
   </sheetData>
@@ -53313,19 +53320,19 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C4EDCD3-948A-4746-BA92-4F40FAE051F5}">
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="23" width="24.26953125" customWidth="1"/>
-    <col min="24" max="24" width="23.7265625" customWidth="1"/>
+    <col min="1" max="23" width="24.28515625" customWidth="1"/>
+    <col min="24" max="24" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -53336,58 +53343,59 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A3" s="3"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D4" t="s">
-        <v>85</v>
-      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="2">
+  <tableParts count="1">
     <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{475BB2F3-1CC8-4BC5-A03F-0361CE5C98B1}">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="23" width="24.28515625" customWidth="1"/>
+    <col min="24" max="24" width="23.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1DB5004-6B6E-472E-AA4A-87F3940EC092}">
   <dimension ref="A1:P4"/>
   <sheetViews>
@@ -53396,21 +53404,21 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.453125" customWidth="1"/>
-    <col min="2" max="2" width="22.7265625" customWidth="1"/>
-    <col min="3" max="3" width="49.36328125" customWidth="1"/>
-    <col min="4" max="4" width="21.453125" customWidth="1"/>
-    <col min="5" max="5" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.54296875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="14.6328125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="14" width="14.54296875" style="1" customWidth="1"/>
-    <col min="15" max="15" width="12.1796875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="36.1796875" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="3" max="3" width="49.42578125" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="14" width="14.5703125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="12.140625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="36.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>24</v>
       </c>
@@ -53426,46 +53434,46 @@
       <c r="E1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="M1" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="N1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="O1" s="9" t="s">
         <v>18</v>
       </c>
       <c r="P1" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A2" s="9"/>
-      <c r="B2" s="12"/>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="8"/>
+      <c r="B2" s="11"/>
       <c r="P2" s="2"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="G3" s="4" t="e">
         <f>SUBTOTAL(101,Table13[Average Duration Microseconds])</f>
         <v>#DIV/0!</v>
@@ -53505,7 +53513,7 @@
       </c>
       <c r="P3" s="2"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>22</v>
       </c>
@@ -53558,59 +53566,59 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="13" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="16" max="20" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="27" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="20" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="27" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="18" bestFit="1" customWidth="1"/>
-    <col min="31" max="35" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="37" max="43" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="45" max="47" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="51" max="52" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="54" max="61" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="63" max="64" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="66" max="68" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="70" max="72" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="75" max="77" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="82" max="92" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="35" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="43" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="45" max="47" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="51" max="52" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="54" max="61" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="63" max="64" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="66" max="68" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="70" max="72" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="75" max="77" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="82" max="92" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>28</v>
       </c>
       <c r="B2" t="s">
@@ -53620,13 +53628,13 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>29</v>
       </c>
     </row>
@@ -53643,23 +53651,23 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>28</v>
       </c>
       <c r="B4" t="s">
@@ -53669,13 +53677,13 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="8" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>29</v>
       </c>
     </row>
@@ -53690,59 +53698,59 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="13" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="16" max="20" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="27" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="20" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="27" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="18" bestFit="1" customWidth="1"/>
-    <col min="31" max="35" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="37" max="43" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="45" max="47" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="51" max="52" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="54" max="61" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="63" max="64" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="66" max="68" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="70" max="72" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="75" max="77" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="82" max="92" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="35" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="43" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="45" max="47" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="51" max="52" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="54" max="61" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="63" max="64" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="66" max="68" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="70" max="72" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="75" max="77" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="82" max="92" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>28</v>
       </c>
       <c r="B2" t="s">
@@ -53752,13 +53760,13 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>29</v>
       </c>
     </row>
@@ -53775,59 +53783,59 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="13" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="16" max="20" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="27" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="20" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="27" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="18" bestFit="1" customWidth="1"/>
-    <col min="31" max="35" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="37" max="43" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="45" max="47" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="51" max="52" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="54" max="61" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="63" max="64" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="66" max="68" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="70" max="72" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="75" max="77" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="82" max="92" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="35" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="43" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="45" max="47" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="51" max="52" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="54" max="61" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="63" max="64" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="66" max="68" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="70" max="72" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="75" max="77" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="82" max="92" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>28</v>
       </c>
       <c r="B2" t="s">
@@ -53837,13 +53845,13 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>29</v>
       </c>
     </row>
@@ -53858,59 +53866,59 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="13" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="16" max="20" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="27" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="20" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="27" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="18" bestFit="1" customWidth="1"/>
-    <col min="31" max="35" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="37" max="43" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="45" max="47" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="51" max="52" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="54" max="61" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="63" max="64" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="66" max="68" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="70" max="72" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="75" max="77" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="82" max="92" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="35" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="43" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="45" max="47" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="51" max="52" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="54" max="61" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="63" max="64" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="66" max="68" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="70" max="72" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="75" max="77" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="82" max="92" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>28</v>
       </c>
       <c r="B2" t="s">
@@ -53920,13 +53928,13 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>29</v>
       </c>
     </row>
@@ -53941,59 +53949,59 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="13" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="16" max="20" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="27" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="20" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="27" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="18" bestFit="1" customWidth="1"/>
-    <col min="31" max="35" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="37" max="43" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="45" max="47" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="51" max="52" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="54" max="61" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="63" max="64" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="66" max="68" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="70" max="72" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="75" max="77" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="82" max="92" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="35" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="43" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="45" max="47" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="51" max="52" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="54" max="61" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="63" max="64" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="66" max="68" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="70" max="72" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="75" max="77" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="82" max="92" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>28</v>
       </c>
       <c r="B2" t="s">
@@ -54003,13 +54011,13 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>29</v>
       </c>
     </row>
@@ -54026,26 +54034,26 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.26953125" customWidth="1"/>
-    <col min="3" max="5" width="31.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="3" max="5" width="31.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
-    <col min="7" max="7" width="7.54296875" customWidth="1"/>
-    <col min="8" max="8" width="13.54296875" customWidth="1"/>
-    <col min="9" max="9" width="19.54296875" customWidth="1"/>
-    <col min="10" max="10" width="17.81640625" customWidth="1"/>
-    <col min="11" max="11" width="17.81640625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="19.1796875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="14.36328125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="17.81640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="13.7265625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="14.6328125" style="1" customWidth="1"/>
-    <col min="17" max="20" width="17.81640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" customWidth="1"/>
+    <col min="9" max="9" width="19.5703125" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" customWidth="1"/>
+    <col min="11" max="11" width="17.85546875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="19.140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="17.85546875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="13.7109375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="14.5703125" style="1" customWidth="1"/>
+    <col min="17" max="20" width="17.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>24</v>
       </c>
@@ -54076,38 +54084,38 @@
       <c r="J1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="M1" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="N1" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="O1" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="P1" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="Q1" s="10" t="s">
+      <c r="Q1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="R1" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="S1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="10" t="s">
+      <c r="T1" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -54178,18 +54186,18 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="23.26953125" customWidth="1"/>
-    <col min="3" max="3" width="38.90625" customWidth="1"/>
-    <col min="4" max="4" width="25.36328125" customWidth="1"/>
-    <col min="5" max="8" width="21.81640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="38.85546875" customWidth="1"/>
+    <col min="4" max="4" width="25.42578125" customWidth="1"/>
+    <col min="5" max="8" width="21.85546875" style="1" customWidth="1"/>
     <col min="9" max="9" width="20" style="1" customWidth="1"/>
-    <col min="10" max="10" width="15.26953125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -54202,18 +54210,18 @@
       <c r="D1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
     </row>
-    <row r="4" spans="1:10" s="2" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>24</v>
       </c>
@@ -54226,173 +54234,173 @@
       <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="J4" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D9" s="4"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D12" s="4"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D13" s="4"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D14" s="4"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D15" s="4"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D16" s="4"/>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17" s="4"/>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D18" s="4"/>
     </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D19" s="4"/>
     </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D20" s="4"/>
     </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D21" s="4"/>
     </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D22" s="4"/>
     </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D23" s="4"/>
     </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D24" s="4"/>
     </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D25" s="4"/>
     </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D26" s="4"/>
     </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D27" s="4"/>
     </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D28" s="4"/>
     </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D29" s="4"/>
     </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D30" s="4"/>
     </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D31" s="4"/>
     </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D32" s="4"/>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D33" s="4"/>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D34" s="4"/>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D35" s="4"/>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D36" s="4"/>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D37" s="4"/>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D38" s="4"/>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D39" s="4"/>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D40" s="4"/>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D41" s="4"/>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D42" s="4"/>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D43" s="4"/>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D44" s="4"/>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D45" s="4"/>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D46" s="4"/>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D47" s="4"/>
     </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D48" s="4"/>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D49" s="4"/>
     </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D50" s="4"/>
     </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D51" s="4"/>
     </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D52" s="4"/>
     </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D53" s="4"/>
     </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D54" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated CPU tab in PerformanceReport.xlsx to include Average CPU %
</commit_message>
<xml_diff>
--- a/QueryStore/SQLServer2016/ExcelTemplates/PerformanceReport.xlsx
+++ b/QueryStore/SQLServer2016/ExcelTemplates/PerformanceReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Version Control\SQLServerPerformanceTuning\QueryStore\SQLServer2016\ExcelTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6EA21B4-E1CF-4DD6-9D46-C3993BC05BAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11039C91-5F86-42D0-A3AF-5DC691FCE9BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{E57F5ADB-DFB2-48C1-AB7B-5552241A8B93}"/>
   </bookViews>
@@ -38,7 +38,7 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="595" r:id="rId19"/>
+    <pivotCache cacheId="638" r:id="rId19"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -232,9 +232,6 @@
     <t>Max Duration Microseconds</t>
   </si>
   <si>
-    <t>Total CPU Hours</t>
-  </si>
-  <si>
     <t>Min CPU Microseconds</t>
   </si>
   <si>
@@ -341,6 +338,9 @@
   </si>
   <si>
     <t>capture_plan_statement</t>
+  </si>
+  <si>
+    <t>Average CPU %</t>
   </si>
 </sst>
 </file>
@@ -48130,7 +48130,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6B74A5C7-4412-4D02-A585-F29DACEC11A2}" name="PivotTable2" cacheId="595" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6B74A5C7-4412-4D02-A585-F29DACEC11A2}" name="PivotTable2" cacheId="638" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7">
   <location ref="A1:C4" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="25">
     <pivotField axis="axisCol" showAll="0">
@@ -48653,7 +48653,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{05205779-AA59-4F6D-B5B7-B5805E83743E}" name="PivotTable5" cacheId="595" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{05205779-AA59-4F6D-B5B7-B5805E83743E}" name="PivotTable5" cacheId="638" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
   <location ref="A3:C6" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="25">
     <pivotField axis="axisCol" showAll="0">
@@ -49167,7 +49167,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{18777F2B-B005-42C4-8BA6-420B837E756F}" name="PivotTable2" cacheId="595" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{18777F2B-B005-42C4-8BA6-420B837E756F}" name="PivotTable2" cacheId="638" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="A1:C4" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="25">
     <pivotField axis="axisCol" showAll="0">
@@ -49678,7 +49678,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A47CD3EC-D199-4326-A3BB-466C9182D620}" name="PivotTable2" cacheId="595" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A47CD3EC-D199-4326-A3BB-466C9182D620}" name="PivotTable2" cacheId="638" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8">
   <location ref="A1:C4" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="25">
     <pivotField axis="axisCol" showAll="0">
@@ -50198,7 +50198,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8950B02F-B669-42A6-B730-5717AEFF6DC1}" name="PivotTable3" cacheId="595" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8950B02F-B669-42A6-B730-5717AEFF6DC1}" name="PivotTable3" cacheId="638" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="A1:C4" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="25">
     <pivotField axis="axisCol" showAll="0">
@@ -50709,7 +50709,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DF2C72FF-63FA-483C-9CB9-93C4252E7C29}" name="PivotTable4" cacheId="595" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DF2C72FF-63FA-483C-9CB9-93C4252E7C29}" name="PivotTable4" cacheId="638" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="A1:C4" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="25">
     <pivotField axis="axisCol" showAll="0">
@@ -51458,7 +51458,7 @@
   <autoFilter ref="A1:D2" xr:uid="{1C5DB8F4-590E-4152-AFFB-249253798EE6}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{9717F265-F67A-49A3-AE04-7B6776C754A4}" name="Total CPU Minutes" dataDxfId="85"/>
-    <tableColumn id="2" xr3:uid="{564E0A27-E07A-4813-B5BD-DC036BC521E5}" name="Total CPU Hours" dataDxfId="84"/>
+    <tableColumn id="2" xr3:uid="{564E0A27-E07A-4813-B5BD-DC036BC521E5}" name="Average CPU %" dataDxfId="84"/>
     <tableColumn id="3" xr3:uid="{BCBE223D-7EB0-4767-A54B-A0D03733547F}" name="Total Query Count"/>
     <tableColumn id="4" xr3:uid="{8B228F54-C51A-4B19-AA58-6C1BEB167D71}" name="Total Query Count for 80% CPU"/>
   </tableColumns>
@@ -51867,13 +51867,13 @@
         <v>13</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E1" s="9"/>
       <c r="F1" s="9"/>
@@ -51903,13 +51903,13 @@
         <v>11</v>
       </c>
       <c r="F4" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="H4" s="9" t="s">
         <v>51</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>52</v>
       </c>
       <c r="I4" s="9" t="s">
         <v>13</v>
@@ -51918,7 +51918,7 @@
         <v>4</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -52158,13 +52158,13 @@
         <v>35</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E1" s="9"/>
       <c r="F1" s="9"/>
@@ -52194,19 +52194,19 @@
         <v>11</v>
       </c>
       <c r="F4" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G4" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="H4" s="9" t="s">
         <v>80</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>81</v>
       </c>
       <c r="I4" s="9" t="s">
         <v>35</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -52401,7 +52401,7 @@
         <v>7</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E1" s="9"/>
       <c r="F1" s="9"/>
@@ -52431,19 +52431,19 @@
         <v>11</v>
       </c>
       <c r="F4" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="H4" s="9" t="s">
         <v>55</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>56</v>
       </c>
       <c r="I4" s="9" t="s">
         <v>14</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -52633,13 +52633,13 @@
         <v>32</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E1" s="9"/>
       <c r="F1" s="9"/>
@@ -52669,19 +52669,19 @@
         <v>11</v>
       </c>
       <c r="F4" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="H4" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>60</v>
       </c>
       <c r="I4" s="9" t="s">
         <v>33</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -52876,7 +52876,7 @@
         <v>7</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E1" s="9"/>
       <c r="F1" s="9"/>
@@ -52906,19 +52906,19 @@
         <v>11</v>
       </c>
       <c r="F4" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="G4" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="H4" s="9" t="s">
         <v>68</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>69</v>
       </c>
       <c r="I4" s="9" t="s">
         <v>16</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -53113,7 +53113,7 @@
         <v>7</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E1" s="9"/>
       <c r="F1" s="9"/>
@@ -53143,19 +53143,19 @@
         <v>11</v>
       </c>
       <c r="F4" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G4" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="H4" s="9" t="s">
         <v>73</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>74</v>
       </c>
       <c r="I4" s="9" t="s">
         <v>18</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -53340,7 +53340,7 @@
         <v>46</v>
       </c>
       <c r="C1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -53380,10 +53380,10 @@
         <v>46</v>
       </c>
       <c r="C1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -53429,7 +53429,7 @@
         <v>9</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>10</v>
@@ -53450,7 +53450,7 @@
         <v>35</v>
       </c>
       <c r="K1" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L1" s="9" t="s">
         <v>14</v>
@@ -53622,7 +53622,7 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2" t="s">
         <v>29</v>
@@ -53630,7 +53630,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -53671,7 +53671,7 @@
         <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C4" t="s">
         <v>29</v>
@@ -53679,7 +53679,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -53754,7 +53754,7 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2" t="s">
         <v>29</v>
@@ -53762,7 +53762,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -53839,7 +53839,7 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2" t="s">
         <v>29</v>
@@ -53847,7 +53847,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -53922,7 +53922,7 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2" t="s">
         <v>29</v>
@@ -53930,7 +53930,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -54005,7 +54005,7 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2" t="s">
         <v>29</v>
@@ -54013,7 +54013,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>